<commit_message>
The Reaper’s Hideout 추가
</commit_message>
<xml_diff>
--- a/islands.xlsx
+++ b/islands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\develop\sotbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9845BE93-4A92-4B6C-949F-2FC4E844F33C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCBDB8A-10DD-418E-AAB9-E9AAD0509319}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="3960" windowWidth="29040" windowHeight="15840" xr2:uid="{57CE9F30-7498-4A6F-A24E-70B9499880AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{57CE9F30-7498-4A6F-A24E-70B9499880AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="187">
   <si>
     <t>Cannon Cove</t>
   </si>
@@ -590,6 +590,14 @@
   </si>
   <si>
     <t>region</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I-12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Reaper’s Hideout</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -954,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6851CCB6-8444-484D-BD9F-A7B9156DF748}">
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1871,32 +1879,32 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>141</v>
+        <v>186</v>
       </c>
       <c r="B83" t="s">
-        <v>142</v>
+        <v>185</v>
       </c>
       <c r="C83" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>38</v>
+        <v>141</v>
       </c>
       <c r="B84" t="s">
-        <v>39</v>
+        <v>142</v>
       </c>
       <c r="C84" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>151</v>
+        <v>38</v>
       </c>
       <c r="B85" t="s">
-        <v>152</v>
+        <v>39</v>
       </c>
       <c r="C85" t="s">
         <v>181</v>
@@ -1904,32 +1912,32 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>26</v>
+        <v>151</v>
       </c>
       <c r="B86" t="s">
-        <v>27</v>
+        <v>152</v>
       </c>
       <c r="C86" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="B87" t="s">
-        <v>150</v>
+        <v>27</v>
       </c>
       <c r="C87" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>108</v>
+        <v>149</v>
       </c>
       <c r="B88" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="C88" t="s">
         <v>181</v>
@@ -1937,29 +1945,40 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="B89" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="C89" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
+        <v>68</v>
+      </c>
+      <c r="B90" t="s">
+        <v>69</v>
+      </c>
+      <c r="C90" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>12</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>13</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C91" t="s">
         <v>179</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C90">
-    <sortCondition ref="A2:A90"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C91">
+    <sortCondition ref="A2:A91"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>